<commit_message>
Updated code; minor changes
</commit_message>
<xml_diff>
--- a/derived_figure_data/figure_heatmap_data.xlsx
+++ b/derived_figure_data/figure_heatmap_data.xlsx
@@ -558,31 +558,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>117.6471329894703</v>
+        <v>110.1924425650476</v>
       </c>
       <c r="C4" t="n">
-        <v>65.58430845177185</v>
+        <v>57.61968623303127</v>
       </c>
       <c r="D4" t="n">
-        <v>36.41541399077323</v>
+        <v>28.57071397669369</v>
       </c>
       <c r="E4" t="n">
-        <v>156.2558737892453</v>
+        <v>146.6577824849572</v>
       </c>
       <c r="F4" t="n">
-        <v>117.9486541605075</v>
+        <v>105.0346491525481</v>
       </c>
       <c r="G4" t="n">
-        <v>109.3842329418925</v>
+        <v>89.24636747292939</v>
       </c>
       <c r="H4" t="n">
-        <v>48.00315623676718</v>
+        <v>44.74227987389258</v>
       </c>
       <c r="I4" t="n">
-        <v>43.38023798353111</v>
+        <v>37.90744074760499</v>
       </c>
       <c r="J4" t="n">
-        <v>30.23385205618408</v>
+        <v>23.40654576238592</v>
       </c>
     </row>
     <row r="5">
@@ -592,31 +592,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>109.7444165861925</v>
+        <v>102.7644435297206</v>
       </c>
       <c r="C5" t="n">
-        <v>31.04933647089214</v>
+        <v>26.84345828237605</v>
       </c>
       <c r="D5" t="n">
-        <v>37.94943748089253</v>
+        <v>29.65288478593351</v>
       </c>
       <c r="E5" t="n">
-        <v>66.57086314742844</v>
+        <v>62.10090426537366</v>
       </c>
       <c r="F5" t="n">
-        <v>88.29815753039578</v>
+        <v>78.05127466886734</v>
       </c>
       <c r="G5" t="n">
-        <v>66.4426598167522</v>
+        <v>53.23110915104286</v>
       </c>
       <c r="H5" t="n">
-        <v>130.6989815901636</v>
+        <v>122.5223478551441</v>
       </c>
       <c r="I5" t="n">
-        <v>116.2100560086197</v>
+        <v>103.3549984148074</v>
       </c>
       <c r="J5" t="n">
-        <v>98.23138352478279</v>
+        <v>79.79541311770743</v>
       </c>
     </row>
     <row r="6">
@@ -626,31 +626,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>58.83954403214781</v>
+        <v>54.83363728295296</v>
       </c>
       <c r="C6" t="n">
-        <v>51.25124479746566</v>
+        <v>44.78260899173166</v>
       </c>
       <c r="D6" t="n">
-        <v>25.1052704863845</v>
+        <v>19.35201095469278</v>
       </c>
       <c r="E6" t="n">
-        <v>191.384549441073</v>
+        <v>179.8877227323921</v>
       </c>
       <c r="F6" t="n">
-        <v>165.001361348168</v>
+        <v>147.8196921941428</v>
       </c>
       <c r="G6" t="n">
-        <v>128.2255932044341</v>
+        <v>105.3261397022424</v>
       </c>
       <c r="H6" t="n">
-        <v>19.76627285669955</v>
+        <v>18.27661095680641</v>
       </c>
       <c r="I6" t="n">
-        <v>35.39674141072813</v>
+        <v>30.68870378326882</v>
       </c>
       <c r="J6" t="n">
-        <v>60.16946034369062</v>
+        <v>47.93796524585264</v>
       </c>
     </row>
     <row r="7">
@@ -660,22 +660,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>58.53976098484049</v>
+        <v>54.55540848014569</v>
       </c>
       <c r="C7" t="n">
-        <v>59.70066637658261</v>
+        <v>52.35766048713711</v>
       </c>
       <c r="D7" t="n">
-        <v>40.37100651736134</v>
+        <v>31.65069767141917</v>
       </c>
       <c r="E7" t="n">
-        <v>108.7939923371728</v>
+        <v>101.8453148663166</v>
       </c>
       <c r="F7" t="n">
-        <v>48.53724674759334</v>
+        <v>42.3885188099509</v>
       </c>
       <c r="G7" t="n">
-        <v>63.29056072302646</v>
+        <v>50.49788787996999</v>
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -688,31 +688,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>47.52414334244763</v>
+        <v>44.23926008865504</v>
       </c>
       <c r="C8" t="n">
-        <v>30.54222635764374</v>
+        <v>26.51350883487405</v>
       </c>
       <c r="D8" t="n">
-        <v>44.67652042119261</v>
+        <v>35.26678825307079</v>
       </c>
       <c r="E8" t="n">
-        <v>132.4838876388025</v>
+        <v>124.1905833069073</v>
       </c>
       <c r="F8" t="n">
-        <v>200.7679214173183</v>
+        <v>180.6037570874865</v>
       </c>
       <c r="G8" t="n">
-        <v>63.24688727068201</v>
+        <v>50.66235340943326</v>
       </c>
       <c r="H8" t="n">
-        <v>33.00000331782438</v>
+        <v>30.653753449433</v>
       </c>
       <c r="I8" t="n">
-        <v>76.78570620011686</v>
+        <v>67.67318381932681</v>
       </c>
       <c r="J8" t="n">
-        <v>70.45318458101363</v>
+        <v>56.45873709437471</v>
       </c>
     </row>
     <row r="9">
@@ -725,22 +725,22 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>460.0310605298783</v>
+        <v>435.2671109601094</v>
       </c>
       <c r="F9" t="n">
-        <v>182.8974118841354</v>
+        <v>164.217904386645</v>
       </c>
       <c r="G9" t="n">
-        <v>172.7562060358902</v>
+        <v>144.0102899073091</v>
       </c>
       <c r="H9" t="n">
-        <v>1164.209100634849</v>
+        <v>1108.691555021345</v>
       </c>
       <c r="I9" t="n">
-        <v>515.4140182636731</v>
+        <v>473.0148269318066</v>
       </c>
       <c r="J9" t="n">
-        <v>517.2866261978332</v>
+        <v>449.6994267145616</v>
       </c>
     </row>
     <row r="10">
@@ -753,13 +753,13 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>152.1996147517976</v>
+        <v>142.8166029394603</v>
       </c>
       <c r="F10" t="n">
-        <v>106.0005371974042</v>
+        <v>94.07402089857567</v>
       </c>
       <c r="G10" t="n">
-        <v>77.74340968010293</v>
+        <v>62.55386590348688</v>
       </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
@@ -773,25 +773,25 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
-        <v>10.52129927579073</v>
+        <v>8.888959440147051</v>
       </c>
       <c r="D11" t="n">
-        <v>8.936838839142068</v>
+        <v>6.582678528844983</v>
       </c>
       <c r="E11" t="n">
-        <v>84.45577424809399</v>
+        <v>78.9106656088516</v>
       </c>
       <c r="F11" t="n">
-        <v>35.37950716907356</v>
+        <v>30.67542962009038</v>
       </c>
       <c r="G11" t="n">
-        <v>41.39676712446624</v>
+        <v>32.48247192495373</v>
       </c>
       <c r="H11" t="n">
-        <v>34.49389817350922</v>
+        <v>32.02074712826816</v>
       </c>
       <c r="I11" t="n">
-        <v>33.91330092959964</v>
+        <v>29.37961730798715</v>
       </c>
       <c r="J11" t="inlineStr"/>
     </row>
@@ -802,31 +802,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>53.15913762191452</v>
+        <v>49.5272862917238</v>
       </c>
       <c r="C12" t="n">
-        <v>50.4184781630188</v>
+        <v>44.04393324572791</v>
       </c>
       <c r="D12" t="n">
-        <v>41.84079073503065</v>
+        <v>32.82394986533163</v>
       </c>
       <c r="E12" t="n">
-        <v>224.0296035422348</v>
+        <v>210.807156840462</v>
       </c>
       <c r="F12" t="n">
-        <v>112.8877353383125</v>
+        <v>100.3359126144678</v>
       </c>
       <c r="G12" t="n">
-        <v>102.0687162417092</v>
+        <v>83.10779193473002</v>
       </c>
       <c r="H12" t="n">
-        <v>25.22888105662514</v>
+        <v>23.3738823020636</v>
       </c>
       <c r="I12" t="n">
-        <v>32.03396767720531</v>
+        <v>27.71300541180904</v>
       </c>
       <c r="J12" t="n">
-        <v>45.53797922153996</v>
+        <v>35.84810000207444</v>
       </c>
     </row>
     <row r="13">
@@ -836,31 +836,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>26.18074569812404</v>
+        <v>24.2624276752935</v>
       </c>
       <c r="C13" t="n">
-        <v>57.73243177035958</v>
+        <v>50.58563556986925</v>
       </c>
       <c r="D13" t="n">
-        <v>63.89534786329467</v>
+        <v>50.99966807793133</v>
       </c>
       <c r="E13" t="n">
-        <v>194.5673363111402</v>
+        <v>182.9099645570676</v>
       </c>
       <c r="F13" t="n">
-        <v>107.8798476070087</v>
+        <v>95.77073544456429</v>
       </c>
       <c r="G13" t="n">
-        <v>65.20230407447738</v>
+        <v>52.13008996610763</v>
       </c>
       <c r="H13" t="n">
-        <v>118.6499066309869</v>
+        <v>111.1347698830379</v>
       </c>
       <c r="I13" t="n">
-        <v>45.38489045605726</v>
+        <v>39.5952519291469</v>
       </c>
       <c r="J13" t="n">
-        <v>83.24143552228725</v>
+        <v>67.20144926757735</v>
       </c>
     </row>
     <row r="14">
@@ -871,28 +871,28 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>18.20360168785097</v>
+        <v>15.57145635992647</v>
       </c>
       <c r="D14" t="n">
-        <v>27.45579587889236</v>
+        <v>21.21863020363624</v>
       </c>
       <c r="E14" t="n">
-        <v>61.88554473810436</v>
+        <v>57.74196188899122</v>
       </c>
       <c r="F14" t="n">
-        <v>31.026468660787</v>
+        <v>26.84651845539537</v>
       </c>
       <c r="G14" t="n">
-        <v>36.11645435621006</v>
+        <v>28.38839333346069</v>
       </c>
       <c r="H14" t="n">
-        <v>32.60803922285341</v>
+        <v>30.25767221645989</v>
       </c>
       <c r="I14" t="n">
-        <v>37.43802202906349</v>
+        <v>32.49493537250761</v>
       </c>
       <c r="J14" t="n">
-        <v>65.73628733663848</v>
+        <v>52.76986207547512</v>
       </c>
     </row>
     <row r="15">
@@ -902,31 +902,31 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>30.94009685157472</v>
+        <v>28.69903060024998</v>
       </c>
       <c r="C15" t="n">
-        <v>42.83300020714464</v>
+        <v>37.37903134754277</v>
       </c>
       <c r="D15" t="n">
-        <v>18.47201887023716</v>
+        <v>14.06641221593484</v>
       </c>
       <c r="E15" t="n">
-        <v>238.7958180752232</v>
+        <v>224.8209797618</v>
       </c>
       <c r="F15" t="n">
-        <v>117.5829613362955</v>
+        <v>104.6035430784413</v>
       </c>
       <c r="G15" t="n">
-        <v>142.4010753524475</v>
+        <v>117.5033140596023</v>
       </c>
       <c r="H15" t="n">
-        <v>99.81205733139194</v>
+        <v>93.47493840586918</v>
       </c>
       <c r="I15" t="n">
-        <v>73.83695258760774</v>
+        <v>65.03093282903967</v>
       </c>
       <c r="J15" t="n">
-        <v>70.41036921372253</v>
+        <v>56.4957246320544</v>
       </c>
     </row>
     <row r="16">
@@ -936,31 +936,31 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>85.19671651090493</v>
+        <v>79.68056015707417</v>
       </c>
       <c r="C16" t="n">
-        <v>79.51348797376616</v>
+        <v>70.13990935080736</v>
       </c>
       <c r="D16" t="n">
-        <v>38.21106283720415</v>
+        <v>29.97117811541586</v>
       </c>
       <c r="E16" t="n">
-        <v>278.2907121763365</v>
+        <v>262.278261637464</v>
       </c>
       <c r="F16" t="n">
-        <v>165.7553817354697</v>
+        <v>148.5130260778394</v>
       </c>
       <c r="G16" t="n">
-        <v>190.2818834073547</v>
+        <v>158.9085031620917</v>
       </c>
       <c r="H16" t="n">
-        <v>63.82232058586972</v>
+        <v>59.56756936635685</v>
       </c>
       <c r="I16" t="n">
-        <v>27.96534396096305</v>
+        <v>24.12349742044306</v>
       </c>
       <c r="J16" t="n">
-        <v>74.70668444360305</v>
+        <v>60.01080398491884</v>
       </c>
     </row>
     <row r="17">
@@ -970,31 +970,31 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>57.71749612937747</v>
+        <v>53.77935998977024</v>
       </c>
       <c r="C17" t="n">
-        <v>29.53762561823682</v>
+        <v>25.50882759738294</v>
       </c>
       <c r="D17" t="n">
-        <v>37.45510123138296</v>
+        <v>29.25085216482291</v>
       </c>
       <c r="E17" t="n">
-        <v>80.12338121368924</v>
+        <v>74.88758081973657</v>
       </c>
       <c r="F17" t="n">
-        <v>90.51602983949834</v>
+        <v>80.06071731720409</v>
       </c>
       <c r="G17" t="n">
-        <v>65.16355487464639</v>
+        <v>52.27483502075336</v>
       </c>
       <c r="H17" t="n">
-        <v>163.2237986580481</v>
+        <v>153.2435822960094</v>
       </c>
       <c r="I17" t="n">
-        <v>67.57713510043939</v>
+        <v>59.40199607386623</v>
       </c>
       <c r="J17" t="n">
-        <v>95.76556547859957</v>
+        <v>77.78778965745687</v>
       </c>
     </row>
     <row r="18">
@@ -1004,31 +1004,31 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>94.68673386039441</v>
+        <v>88.5854842925591</v>
       </c>
       <c r="C18" t="n">
-        <v>72.76203338898242</v>
+        <v>64.05640379474839</v>
       </c>
       <c r="D18" t="n">
-        <v>109.35639509151</v>
+        <v>89.22176253546256</v>
       </c>
       <c r="E18" t="n">
-        <v>363.8754885834794</v>
+        <v>343.6033712278563</v>
       </c>
       <c r="F18" t="n">
-        <v>212.9455266754034</v>
+        <v>191.8398303522782</v>
       </c>
       <c r="G18" t="n">
-        <v>174.6574375965811</v>
+        <v>145.2853350342348</v>
       </c>
       <c r="H18" t="n">
-        <v>29.16542275627078</v>
+        <v>27.04132108912641</v>
       </c>
       <c r="I18" t="n">
-        <v>29.74145061955872</v>
+        <v>25.68855354141774</v>
       </c>
       <c r="J18" t="n">
-        <v>71.38441114392371</v>
+        <v>57.51257332150868</v>
       </c>
     </row>
     <row r="19">
@@ -1038,26 +1038,26 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>41.84456044495871</v>
+        <v>38.89868095070408</v>
       </c>
       <c r="C19" t="n">
-        <v>32.0012762138772</v>
+        <v>27.6835091677908</v>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
-        <v>74.98357591163813</v>
+        <v>70.00458771494738</v>
       </c>
       <c r="F19" t="n">
-        <v>69.26659143516761</v>
+        <v>60.91482879581577</v>
       </c>
       <c r="G19" t="n">
-        <v>37.49994681571157</v>
+        <v>29.29283111417643</v>
       </c>
       <c r="H19" t="n">
-        <v>96.93648423924066</v>
+        <v>90.66245162087684</v>
       </c>
       <c r="I19" t="n">
-        <v>36.66287041695735</v>
+        <v>31.807976274071</v>
       </c>
       <c r="J19" t="inlineStr"/>
     </row>
@@ -1068,31 +1068,31 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>128.9256207072849</v>
+        <v>120.8614520128894</v>
       </c>
       <c r="C20" t="n">
-        <v>95.83998393514813</v>
+        <v>84.93758515710877</v>
       </c>
       <c r="D20" t="n">
-        <v>63.89670325289727</v>
+        <v>51.00084005992032</v>
       </c>
       <c r="E20" t="n">
-        <v>282.9493166001197</v>
+        <v>266.7514101370975</v>
       </c>
       <c r="F20" t="n">
-        <v>103.3549194350547</v>
+        <v>91.7358843933454</v>
       </c>
       <c r="G20" t="n">
-        <v>136.0349663010389</v>
+        <v>112.5236844983666</v>
       </c>
       <c r="H20" t="n">
-        <v>64.2651872408465</v>
+        <v>60.03218916151308</v>
       </c>
       <c r="I20" t="n">
-        <v>70.4160441813828</v>
+        <v>61.96462226368543</v>
       </c>
       <c r="J20" t="n">
-        <v>71.64288452818573</v>
+        <v>57.47619290868154</v>
       </c>
     </row>
     <row r="21">
@@ -1102,31 +1102,31 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>49.83411815638158</v>
+        <v>46.42451271212873</v>
       </c>
       <c r="C21" t="n">
-        <v>51.93618091643371</v>
+        <v>45.41024134071904</v>
       </c>
       <c r="D21" t="n">
-        <v>28.12195865491273</v>
+        <v>21.70657722237194</v>
       </c>
       <c r="E21" t="n">
-        <v>345.7089924415055</v>
+        <v>326.3308823576667</v>
       </c>
       <c r="F21" t="n">
-        <v>152.8166275795765</v>
+        <v>136.680623540596</v>
       </c>
       <c r="G21" t="n">
-        <v>168.0547798591772</v>
+        <v>139.5572797545771</v>
       </c>
       <c r="H21" t="n">
-        <v>38.4340182520739</v>
+        <v>35.72189683712494</v>
       </c>
       <c r="I21" t="n">
-        <v>38.60908470952823</v>
+        <v>33.59731088589378</v>
       </c>
       <c r="J21" t="n">
-        <v>51.87390482308141</v>
+        <v>41.0535976918815</v>
       </c>
     </row>
     <row r="22">
@@ -1136,31 +1136,31 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>232.8171295598836</v>
+        <v>219.1356882701513</v>
       </c>
       <c r="C22" t="n">
-        <v>162.2351331702462</v>
+        <v>145.3126682716008</v>
       </c>
       <c r="D22" t="n">
-        <v>191.0081696788698</v>
+        <v>159.9161716648773</v>
       </c>
       <c r="E22" t="n">
-        <v>551.286027798512</v>
+        <v>522.1626674214552</v>
       </c>
       <c r="F22" t="n">
-        <v>355.5223676284716</v>
+        <v>323.7220137272893</v>
       </c>
       <c r="G22" t="n">
-        <v>176.715794820525</v>
+        <v>147.0597407012749</v>
       </c>
       <c r="H22" t="n">
-        <v>226.8822246575072</v>
+        <v>213.5102549638463</v>
       </c>
       <c r="I22" t="n">
-        <v>100.62136806299</v>
+        <v>89.24134835043893</v>
       </c>
       <c r="J22" t="n">
-        <v>170.6194014288646</v>
+        <v>141.7678192909507</v>
       </c>
     </row>
   </sheetData>
@@ -1283,7 +1283,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>11.07868589835245</v>
+        <v>13.51281341043541</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -1300,10 +1300,10 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>16.25103527233635</v>
+        <v>12.29277085197422</v>
       </c>
       <c r="D5" t="n">
-        <v>11.4815669458481</v>
+        <v>13.98388912944851</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
@@ -1335,13 +1335,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>434.4636350076696</v>
+        <v>370.8270025659695</v>
       </c>
       <c r="C7" t="n">
-        <v>160.4813360763181</v>
+        <v>133.44609246047</v>
       </c>
       <c r="D7" t="n">
-        <v>190.4033730777801</v>
+        <v>209.1969015103554</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -1357,20 +1357,20 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>31.75887694020749</v>
+        <v>24.17969913751245</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>13.76999623982523</v>
+        <v>16.68300682427972</v>
       </c>
       <c r="E8" t="n">
-        <v>43.15808028342339</v>
+        <v>33.35744436084349</v>
       </c>
       <c r="F8" t="n">
-        <v>15.89130495900355</v>
+        <v>12.00963109040615</v>
       </c>
       <c r="G8" t="n">
-        <v>17.78824125425479</v>
+        <v>21.33295935472071</v>
       </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
@@ -1383,20 +1383,20 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>145.8607838018135</v>
+        <v>118.6620610896119</v>
       </c>
       <c r="C9" t="n">
-        <v>109.9925260124897</v>
+        <v>90.01094787188312</v>
       </c>
       <c r="D9" t="n">
-        <v>37.18773519227194</v>
+        <v>43.36825332603961</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>30.60530342172077</v>
+        <v>23.76590005523448</v>
       </c>
       <c r="G9" t="n">
-        <v>19.78253422288658</v>
+        <v>23.63609830609418</v>
       </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
@@ -1409,13 +1409,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>59.95087490619405</v>
+        <v>46.9093695429431</v>
       </c>
       <c r="C10" t="n">
-        <v>41.64378721782447</v>
+        <v>32.77184740227874</v>
       </c>
       <c r="D10" t="n">
-        <v>22.00511003893284</v>
+        <v>26.19911881840072</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
@@ -1447,22 +1447,22 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>43.62791462660922</v>
+        <v>33.66069654838154</v>
       </c>
       <c r="C12" t="n">
-        <v>24.65839732328959</v>
+        <v>19.04427616104488</v>
       </c>
       <c r="D12" t="n">
-        <v>11.36305247859167</v>
+        <v>13.84979898043263</v>
       </c>
       <c r="E12" t="n">
-        <v>35.13401704798311</v>
+        <v>26.86449712505085</v>
       </c>
       <c r="F12" t="n">
-        <v>24.372441065972</v>
+        <v>18.75869170158835</v>
       </c>
       <c r="G12" t="n">
-        <v>21.73571566293445</v>
+        <v>25.8606030994233</v>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
@@ -1507,13 +1507,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>89.23366009177978</v>
+        <v>71.04424354908387</v>
       </c>
       <c r="C15" t="n">
-        <v>34.06118319332041</v>
+        <v>26.60934968187004</v>
       </c>
       <c r="D15" t="n">
-        <v>29.54454156275628</v>
+        <v>34.62851324205592</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
@@ -1529,19 +1529,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>45.96891476271058</v>
+        <v>35.60556076029869</v>
       </c>
       <c r="C16" t="n">
-        <v>43.18449768932373</v>
+        <v>34.11426873374684</v>
       </c>
       <c r="D16" t="n">
-        <v>20.971376637569</v>
+        <v>25.01307611131964</v>
       </c>
       <c r="E16" t="n">
-        <v>28.77107985648692</v>
+        <v>21.79605566806631</v>
       </c>
       <c r="F16" t="n">
-        <v>23.77639674995053</v>
+        <v>18.26803393438589</v>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
@@ -1571,13 +1571,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>61.32135631964412</v>
+        <v>48.50297244336296</v>
       </c>
       <c r="C18" t="n">
-        <v>21.88837984738793</v>
+        <v>16.77317457822999</v>
       </c>
       <c r="D18" t="n">
-        <v>31.29901669278033</v>
+        <v>36.73050359626844</v>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
@@ -1641,13 +1641,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>42.41069700472188</v>
+        <v>32.86854842011829</v>
       </c>
       <c r="C22" t="n">
-        <v>16.37274595610389</v>
+        <v>12.38862648048871</v>
       </c>
       <c r="D22" t="n">
-        <v>36.22776532739468</v>
+        <v>42.33822035683203</v>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
@@ -1774,31 +1774,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>117.6471329894703</v>
+        <v>110.1924425650476</v>
       </c>
       <c r="C4" t="n">
-        <v>65.58430845177185</v>
+        <v>57.61968623303127</v>
       </c>
       <c r="D4" t="n">
-        <v>47.49409988912568</v>
+        <v>42.0835273871291</v>
       </c>
       <c r="E4" t="n">
-        <v>156.2558737892453</v>
+        <v>146.6577824849572</v>
       </c>
       <c r="F4" t="n">
-        <v>117.9486541605075</v>
+        <v>105.0346491525481</v>
       </c>
       <c r="G4" t="n">
-        <v>109.3842329418925</v>
+        <v>89.24636747292939</v>
       </c>
       <c r="H4" t="n">
-        <v>48.00315623676718</v>
+        <v>44.74227987389258</v>
       </c>
       <c r="I4" t="n">
-        <v>43.38023798353111</v>
+        <v>37.90744074760499</v>
       </c>
       <c r="J4" t="n">
-        <v>30.23385205618408</v>
+        <v>23.40654576238592</v>
       </c>
     </row>
     <row r="5">
@@ -1808,31 +1808,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>109.7444165861925</v>
+        <v>102.7644435297206</v>
       </c>
       <c r="C5" t="n">
-        <v>47.30037174322849</v>
+        <v>39.13622913435027</v>
       </c>
       <c r="D5" t="n">
-        <v>49.43100442674063</v>
+        <v>43.63677391538202</v>
       </c>
       <c r="E5" t="n">
-        <v>66.57086314742844</v>
+        <v>62.10090426537366</v>
       </c>
       <c r="F5" t="n">
-        <v>88.29815753039578</v>
+        <v>78.05127466886734</v>
       </c>
       <c r="G5" t="n">
-        <v>66.4426598167522</v>
+        <v>53.23110915104286</v>
       </c>
       <c r="H5" t="n">
-        <v>130.6989815901636</v>
+        <v>122.5223478551441</v>
       </c>
       <c r="I5" t="n">
-        <v>116.2100560086197</v>
+        <v>103.3549984148074</v>
       </c>
       <c r="J5" t="n">
-        <v>98.23138352478279</v>
+        <v>79.79541311770743</v>
       </c>
     </row>
     <row r="6">
@@ -1842,31 +1842,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>58.83954403214781</v>
+        <v>54.83363728295296</v>
       </c>
       <c r="C6" t="n">
-        <v>51.25124479746566</v>
+        <v>44.78260899173166</v>
       </c>
       <c r="D6" t="n">
-        <v>25.1052704863845</v>
+        <v>19.35201095469278</v>
       </c>
       <c r="E6" t="n">
-        <v>191.384549441073</v>
+        <v>179.8877227323921</v>
       </c>
       <c r="F6" t="n">
-        <v>165.001361348168</v>
+        <v>147.8196921941428</v>
       </c>
       <c r="G6" t="n">
-        <v>128.2255932044341</v>
+        <v>105.3261397022424</v>
       </c>
       <c r="H6" t="n">
-        <v>19.76627285669955</v>
+        <v>18.27661095680641</v>
       </c>
       <c r="I6" t="n">
-        <v>35.39674141072813</v>
+        <v>30.68870378326882</v>
       </c>
       <c r="J6" t="n">
-        <v>60.16946034369062</v>
+        <v>47.93796524585264</v>
       </c>
     </row>
     <row r="7">
@@ -1876,22 +1876,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>493.00339599251</v>
+        <v>425.3824110461151</v>
       </c>
       <c r="C7" t="n">
-        <v>220.1820024529007</v>
+        <v>185.8037529476071</v>
       </c>
       <c r="D7" t="n">
-        <v>230.7743795951415</v>
+        <v>240.8475991817746</v>
       </c>
       <c r="E7" t="n">
-        <v>108.7939923371728</v>
+        <v>101.8453148663166</v>
       </c>
       <c r="F7" t="n">
-        <v>48.53724674759334</v>
+        <v>42.3885188099509</v>
       </c>
       <c r="G7" t="n">
-        <v>63.29056072302646</v>
+        <v>50.49788787996999</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1910,31 +1910,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>79.28302028265512</v>
+        <v>68.41895922616749</v>
       </c>
       <c r="C8" t="n">
-        <v>30.54222635764374</v>
+        <v>26.51350883487405</v>
       </c>
       <c r="D8" t="n">
-        <v>58.44651666101784</v>
+        <v>51.94979507735051</v>
       </c>
       <c r="E8" t="n">
-        <v>175.6419679222259</v>
+        <v>157.5480276677508</v>
       </c>
       <c r="F8" t="n">
-        <v>216.6592263763219</v>
+        <v>192.6133881778927</v>
       </c>
       <c r="G8" t="n">
-        <v>81.03512852493679</v>
+        <v>71.99531276415397</v>
       </c>
       <c r="H8" t="n">
-        <v>33.00000331782438</v>
+        <v>30.653753449433</v>
       </c>
       <c r="I8" t="n">
-        <v>76.78570620011686</v>
+        <v>67.67318381932681</v>
       </c>
       <c r="J8" t="n">
-        <v>70.45318458101363</v>
+        <v>56.45873709437471</v>
       </c>
     </row>
     <row r="9">
@@ -1944,31 +1944,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>145.8607838018135</v>
+        <v>118.6620610896119</v>
       </c>
       <c r="C9" t="n">
-        <v>109.9925260124897</v>
+        <v>90.01094787188312</v>
       </c>
       <c r="D9" t="n">
-        <v>37.18773519227194</v>
+        <v>43.36825332603961</v>
       </c>
       <c r="E9" t="n">
-        <v>460.0310605298783</v>
+        <v>435.2671109601094</v>
       </c>
       <c r="F9" t="n">
-        <v>213.5027153058561</v>
+        <v>187.9838044418795</v>
       </c>
       <c r="G9" t="n">
-        <v>192.5387402587767</v>
+        <v>167.6463882134033</v>
       </c>
       <c r="H9" t="n">
-        <v>1164.209100634849</v>
+        <v>1108.691555021345</v>
       </c>
       <c r="I9" t="n">
-        <v>515.4140182636731</v>
+        <v>473.0148269318066</v>
       </c>
       <c r="J9" t="n">
-        <v>517.2866261978332</v>
+        <v>449.6994267145616</v>
       </c>
     </row>
     <row r="10">
@@ -1978,22 +1978,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>59.95087490619405</v>
+        <v>46.9093695429431</v>
       </c>
       <c r="C10" t="n">
-        <v>41.64378721782447</v>
+        <v>32.77184740227874</v>
       </c>
       <c r="D10" t="n">
-        <v>22.00511003893284</v>
+        <v>26.19911881840072</v>
       </c>
       <c r="E10" t="n">
-        <v>152.1996147517976</v>
+        <v>142.8166029394603</v>
       </c>
       <c r="F10" t="n">
-        <v>106.0005371974042</v>
+        <v>94.07402089857567</v>
       </c>
       <c r="G10" t="n">
-        <v>77.74340968010293</v>
+        <v>62.55386590348688</v>
       </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
@@ -2009,25 +2009,25 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>10.52129927579073</v>
+        <v>8.888959440147051</v>
       </c>
       <c r="D11" t="n">
-        <v>8.936838839142068</v>
+        <v>6.582678528844983</v>
       </c>
       <c r="E11" t="n">
-        <v>84.45577424809399</v>
+        <v>78.9106656088516</v>
       </c>
       <c r="F11" t="n">
-        <v>35.37950716907356</v>
+        <v>30.67542962009038</v>
       </c>
       <c r="G11" t="n">
-        <v>41.39676712446624</v>
+        <v>32.48247192495373</v>
       </c>
       <c r="H11" t="n">
-        <v>34.49389817350922</v>
+        <v>32.02074712826816</v>
       </c>
       <c r="I11" t="n">
-        <v>33.91330092959964</v>
+        <v>29.37961730798715</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
@@ -2040,31 +2040,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>96.78705224852374</v>
+        <v>83.18798284010535</v>
       </c>
       <c r="C12" t="n">
-        <v>75.0768754863084</v>
+        <v>63.08820940677279</v>
       </c>
       <c r="D12" t="n">
-        <v>53.20384321362232</v>
+        <v>46.67374884576427</v>
       </c>
       <c r="E12" t="n">
-        <v>259.1636205902179</v>
+        <v>237.6716539655128</v>
       </c>
       <c r="F12" t="n">
-        <v>137.2601764042846</v>
+        <v>119.0946043160561</v>
       </c>
       <c r="G12" t="n">
-        <v>123.8044319046437</v>
+        <v>108.9683950341533</v>
       </c>
       <c r="H12" t="n">
-        <v>25.22888105662514</v>
+        <v>23.3738823020636</v>
       </c>
       <c r="I12" t="n">
-        <v>32.03396767720531</v>
+        <v>27.71300541180904</v>
       </c>
       <c r="J12" t="n">
-        <v>45.53797922153996</v>
+        <v>35.84810000207444</v>
       </c>
     </row>
     <row r="13">
@@ -2074,31 +2074,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>26.18074569812404</v>
+        <v>24.2624276752935</v>
       </c>
       <c r="C13" t="n">
-        <v>57.73243177035958</v>
+        <v>50.58563556986925</v>
       </c>
       <c r="D13" t="n">
-        <v>63.89534786329467</v>
+        <v>50.99966807793133</v>
       </c>
       <c r="E13" t="n">
-        <v>194.5673363111402</v>
+        <v>182.9099645570676</v>
       </c>
       <c r="F13" t="n">
-        <v>107.8798476070087</v>
+        <v>95.77073544456429</v>
       </c>
       <c r="G13" t="n">
-        <v>65.20230407447738</v>
+        <v>52.13008996610763</v>
       </c>
       <c r="H13" t="n">
-        <v>118.6499066309869</v>
+        <v>111.1347698830379</v>
       </c>
       <c r="I13" t="n">
-        <v>45.38489045605726</v>
+        <v>39.5952519291469</v>
       </c>
       <c r="J13" t="n">
-        <v>83.24143552228725</v>
+        <v>67.20144926757735</v>
       </c>
     </row>
     <row r="14">
@@ -2111,28 +2111,28 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>18.20360168785097</v>
+        <v>15.57145635992647</v>
       </c>
       <c r="D14" t="n">
-        <v>27.45579587889236</v>
+        <v>21.21863020363624</v>
       </c>
       <c r="E14" t="n">
-        <v>61.88554473810436</v>
+        <v>57.74196188899122</v>
       </c>
       <c r="F14" t="n">
-        <v>31.026468660787</v>
+        <v>26.84651845539537</v>
       </c>
       <c r="G14" t="n">
-        <v>36.11645435621006</v>
+        <v>28.38839333346069</v>
       </c>
       <c r="H14" t="n">
-        <v>32.60803922285341</v>
+        <v>30.25767221645989</v>
       </c>
       <c r="I14" t="n">
-        <v>37.43802202906349</v>
+        <v>32.49493537250761</v>
       </c>
       <c r="J14" t="n">
-        <v>65.73628733663848</v>
+        <v>52.76986207547512</v>
       </c>
     </row>
     <row r="15">
@@ -2142,31 +2142,31 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>120.1737569433545</v>
+        <v>99.74327414933386</v>
       </c>
       <c r="C15" t="n">
-        <v>76.89418340046504</v>
+        <v>63.98838102941281</v>
       </c>
       <c r="D15" t="n">
-        <v>48.01656043299344</v>
+        <v>48.69492545799076</v>
       </c>
       <c r="E15" t="n">
-        <v>238.7958180752232</v>
+        <v>224.8209797618</v>
       </c>
       <c r="F15" t="n">
-        <v>117.5829613362955</v>
+        <v>104.6035430784413</v>
       </c>
       <c r="G15" t="n">
-        <v>142.4010753524475</v>
+        <v>117.5033140596023</v>
       </c>
       <c r="H15" t="n">
-        <v>99.81205733139194</v>
+        <v>93.47493840586918</v>
       </c>
       <c r="I15" t="n">
-        <v>73.83695258760774</v>
+        <v>65.03093282903967</v>
       </c>
       <c r="J15" t="n">
-        <v>70.41036921372253</v>
+        <v>56.4957246320544</v>
       </c>
     </row>
     <row r="16">
@@ -2176,31 +2176,31 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>131.1656312736155</v>
+        <v>115.2861209173729</v>
       </c>
       <c r="C16" t="n">
-        <v>122.6979856630899</v>
+        <v>104.2541780845542</v>
       </c>
       <c r="D16" t="n">
-        <v>59.18243947477315</v>
+        <v>54.98425422673549</v>
       </c>
       <c r="E16" t="n">
-        <v>307.0617920328233</v>
+        <v>284.0743173055303</v>
       </c>
       <c r="F16" t="n">
-        <v>189.5317784854202</v>
+        <v>166.7810600122253</v>
       </c>
       <c r="G16" t="n">
-        <v>190.2818834073547</v>
+        <v>158.9085031620917</v>
       </c>
       <c r="H16" t="n">
-        <v>63.82232058586972</v>
+        <v>59.56756936635685</v>
       </c>
       <c r="I16" t="n">
-        <v>27.96534396096305</v>
+        <v>24.12349742044306</v>
       </c>
       <c r="J16" t="n">
-        <v>74.70668444360305</v>
+        <v>60.01080398491884</v>
       </c>
     </row>
     <row r="17">
@@ -2210,31 +2210,31 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>57.71749612937747</v>
+        <v>53.77935998977024</v>
       </c>
       <c r="C17" t="n">
-        <v>29.53762561823682</v>
+        <v>25.50882759738294</v>
       </c>
       <c r="D17" t="n">
-        <v>37.45510123138296</v>
+        <v>29.25085216482291</v>
       </c>
       <c r="E17" t="n">
-        <v>80.12338121368924</v>
+        <v>74.88758081973657</v>
       </c>
       <c r="F17" t="n">
-        <v>90.51602983949834</v>
+        <v>80.06071731720409</v>
       </c>
       <c r="G17" t="n">
-        <v>65.16355487464639</v>
+        <v>52.27483502075336</v>
       </c>
       <c r="H17" t="n">
-        <v>163.2237986580481</v>
+        <v>153.2435822960094</v>
       </c>
       <c r="I17" t="n">
-        <v>67.57713510043939</v>
+        <v>59.40199607386623</v>
       </c>
       <c r="J17" t="n">
-        <v>95.76556547859957</v>
+        <v>77.78778965745687</v>
       </c>
     </row>
     <row r="18">
@@ -2244,31 +2244,31 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>156.0080901800385</v>
+        <v>137.0884567359221</v>
       </c>
       <c r="C18" t="n">
-        <v>94.65041323637035</v>
+        <v>80.82957837297838</v>
       </c>
       <c r="D18" t="n">
-        <v>140.6554117842903</v>
+        <v>125.952266131731</v>
       </c>
       <c r="E18" t="n">
-        <v>363.8754885834794</v>
+        <v>343.6033712278563</v>
       </c>
       <c r="F18" t="n">
-        <v>212.9455266754034</v>
+        <v>191.8398303522782</v>
       </c>
       <c r="G18" t="n">
-        <v>174.6574375965811</v>
+        <v>145.2853350342348</v>
       </c>
       <c r="H18" t="n">
-        <v>29.16542275627078</v>
+        <v>27.04132108912641</v>
       </c>
       <c r="I18" t="n">
-        <v>29.74145061955872</v>
+        <v>25.68855354141774</v>
       </c>
       <c r="J18" t="n">
-        <v>71.38441114392371</v>
+        <v>57.51257332150868</v>
       </c>
     </row>
     <row r="19">
@@ -2278,28 +2278,28 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>41.84456044495871</v>
+        <v>38.89868095070408</v>
       </c>
       <c r="C19" t="n">
-        <v>32.0012762138772</v>
+        <v>27.6835091677908</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>74.98357591163813</v>
+        <v>70.00458771494738</v>
       </c>
       <c r="F19" t="n">
-        <v>69.26659143516761</v>
+        <v>60.91482879581577</v>
       </c>
       <c r="G19" t="n">
-        <v>37.49994681571157</v>
+        <v>29.29283111417643</v>
       </c>
       <c r="H19" t="n">
-        <v>96.93648423924066</v>
+        <v>90.66245162087684</v>
       </c>
       <c r="I19" t="n">
-        <v>36.66287041695735</v>
+        <v>31.807976274071</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -2312,31 +2312,31 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>128.9256207072849</v>
+        <v>120.8614520128894</v>
       </c>
       <c r="C20" t="n">
-        <v>95.83998393514813</v>
+        <v>84.93758515710877</v>
       </c>
       <c r="D20" t="n">
-        <v>63.89670325289727</v>
+        <v>51.00084005992032</v>
       </c>
       <c r="E20" t="n">
-        <v>282.9493166001197</v>
+        <v>266.7514101370975</v>
       </c>
       <c r="F20" t="n">
-        <v>103.3549194350547</v>
+        <v>91.7358843933454</v>
       </c>
       <c r="G20" t="n">
-        <v>136.0349663010389</v>
+        <v>112.5236844983666</v>
       </c>
       <c r="H20" t="n">
-        <v>64.2651872408465</v>
+        <v>60.03218916151308</v>
       </c>
       <c r="I20" t="n">
-        <v>70.4160441813828</v>
+        <v>61.96462226368543</v>
       </c>
       <c r="J20" t="n">
-        <v>71.64288452818573</v>
+        <v>57.47619290868154</v>
       </c>
     </row>
     <row r="21">
@@ -2346,31 +2346,31 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>49.83411815638158</v>
+        <v>46.42451271212873</v>
       </c>
       <c r="C21" t="n">
-        <v>51.93618091643371</v>
+        <v>45.41024134071904</v>
       </c>
       <c r="D21" t="n">
-        <v>28.12195865491273</v>
+        <v>21.70657722237194</v>
       </c>
       <c r="E21" t="n">
-        <v>345.7089924415055</v>
+        <v>326.3308823576667</v>
       </c>
       <c r="F21" t="n">
-        <v>152.8166275795765</v>
+        <v>136.680623540596</v>
       </c>
       <c r="G21" t="n">
-        <v>168.0547798591772</v>
+        <v>139.5572797545771</v>
       </c>
       <c r="H21" t="n">
-        <v>38.4340182520739</v>
+        <v>35.72189683712494</v>
       </c>
       <c r="I21" t="n">
-        <v>38.60908470952823</v>
+        <v>33.59731088589378</v>
       </c>
       <c r="J21" t="n">
-        <v>51.87390482308141</v>
+        <v>41.0535976918815</v>
       </c>
     </row>
     <row r="22">
@@ -2380,31 +2380,31 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>275.2278265646055</v>
+        <v>252.0042366902696</v>
       </c>
       <c r="C22" t="n">
-        <v>178.6078791263501</v>
+        <v>157.7012947520895</v>
       </c>
       <c r="D22" t="n">
-        <v>227.2359350062644</v>
+        <v>202.2543920217093</v>
       </c>
       <c r="E22" t="n">
-        <v>551.286027798512</v>
+        <v>522.1626674214552</v>
       </c>
       <c r="F22" t="n">
-        <v>355.5223676284716</v>
+        <v>323.7220137272893</v>
       </c>
       <c r="G22" t="n">
-        <v>176.715794820525</v>
+        <v>147.0597407012749</v>
       </c>
       <c r="H22" t="n">
-        <v>226.8822246575072</v>
+        <v>213.5102549638463</v>
       </c>
       <c r="I22" t="n">
-        <v>100.62136806299</v>
+        <v>89.24134835043893</v>
       </c>
       <c r="J22" t="n">
-        <v>170.6194014288646</v>
+        <v>141.7678192909507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>